<commit_message>
Simulador en su version 1.0 esta listo (faltan preguntas adicionales despues del simulador). SliderB5B6 se ajusta a parametros que indican ancho y alto de slider. Se corriegieron problemas en CSV. Cuando la pantalla es menor a 1100 px de ancho ocupara el 100% del ancho.
</commit_message>
<xml_diff>
--- a/data/Estado de Resultados Mx .xlsx
+++ b/data/Estado de Resultados Mx .xlsx
@@ -45,14 +45,6 @@
   <si>
     <t>Numero de clientes 
 Vencidos+4</t>
-  </si>
-  <si>
-    <t>Numero de clientes 
-Saldados015</t>
-  </si>
-  <si>
-    <t>Numero de clientes 
-Saldados+15</t>
   </si>
   <si>
     <t>Numero de clientes 
@@ -230,13 +222,21 @@
     <t>Venta 
 De contado</t>
   </si>
+  <si>
+    <t>Numero de clientes 
+Saldado015</t>
+  </si>
+  <si>
+    <t>Numero de clientes 
+Saldado+15</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -722,7 +722,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1067,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AW1" sqref="AW1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,142 +1107,142 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="BA1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="BB1" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:54" x14ac:dyDescent="0.25">

</xml_diff>